<commit_message>
working on get internal format
</commit_message>
<xml_diff>
--- a/data/basic_info.xlsx
+++ b/data/basic_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\trading_plan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D902CD-BED9-4A09-AE49-3E5436BDC9C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3375D67-253F-4ABE-A3FA-07A5ED5C0B46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28590" tabRatio="733" activeTab="1" xr2:uid="{855E00D3-25C3-4BB2-A61F-0D95BB1AF006}"/>
+    <workbookView xWindow="1500" yWindow="8835" windowWidth="13860" windowHeight="10065" tabRatio="733" activeTab="1" xr2:uid="{855E00D3-25C3-4BB2-A61F-0D95BB1AF006}"/>
   </bookViews>
   <sheets>
     <sheet name="acct_info" sheetId="1" r:id="rId1"/>
@@ -7610,10 +7610,10 @@
   <dimension ref="A1:K133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I61" sqref="I61"/>
+      <selection pane="bottomRight" activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -8508,7 +8508,7 @@
         <v>615</v>
       </c>
       <c r="H32" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I32" t="s">
         <v>978</v>
@@ -8540,7 +8540,7 @@
         <v>931</v>
       </c>
       <c r="H33" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33" t="s">
         <v>979</v>
@@ -8572,7 +8572,7 @@
         <v>720</v>
       </c>
       <c r="H34" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34" t="s">
         <v>1019</v>

</xml_diff>

<commit_message>
update patch data: capital
</commit_message>
<xml_diff>
--- a/data/basic_info.xlsx
+++ b/data/basic_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\trading_plan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3375D67-253F-4ABE-A3FA-07A5ED5C0B46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4CC26A-202F-4FCE-A3FE-7119BC1AC5E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="8835" windowWidth="13860" windowHeight="10065" tabRatio="733" activeTab="1" xr2:uid="{855E00D3-25C3-4BB2-A61F-0D95BB1AF006}"/>
+    <workbookView xWindow="375" yWindow="9630" windowWidth="13860" windowHeight="10065" tabRatio="733" activeTab="1" xr2:uid="{855E00D3-25C3-4BB2-A61F-0D95BB1AF006}"/>
   </bookViews>
   <sheets>
     <sheet name="acct_info" sheetId="1" r:id="rId1"/>
@@ -3856,12 +3856,6 @@
     <t>(905_m_huat_5729.txt,905_m_huat_5729.txt,)</t>
   </si>
   <si>
-    <t>(906_c_gtja_1979.csv,906_c_gtja_1979.csv,)</t>
-  </si>
-  <si>
-    <t>(906_m_gtja_6560.csv,906_m_gtja_6560.csv,)</t>
-  </si>
-  <si>
     <t>(907_c_huat_5588.txt,907_c_huat_5588.txt,)</t>
   </si>
   <si>
@@ -3895,12 +3889,6 @@
     <t>(920_m_huat_1372.txt,920_m_huat_1372.txt,)</t>
   </si>
   <si>
-    <t>(922_c_gtja_0808.csv,922_c_gtja_0808.csv,)</t>
-  </si>
-  <si>
-    <t>(922_m_gtja_7038.csv,922_m_gtja_7038.csv,)</t>
-  </si>
-  <si>
     <t>(930_c_hf_1818.txt,930_c_hf_1818.txt,)</t>
   </si>
   <si>
@@ -4033,6 +4021,22 @@
   </si>
   <si>
     <t>(925_c_hait_1601.xlsx,925_c_hait_1601.xlsx,)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(906_c_gtja_1979.xls,906_c_gtja_1979.xls,)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(906_m_gtja_6560.xls,906_m_gtja_6560.xls,)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(922_c_gtja_0808.xls,922_c_gtja_0808.xls,)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(922_m_gtja_7038.xls,922_m_gtja_7038.xls,)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -7610,10 +7614,10 @@
   <dimension ref="A1:K133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F36" sqref="F36"/>
+      <selection pane="bottomRight" activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7636,10 +7640,10 @@
         <v>899</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>993</v>
+        <v>989</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>994</v>
+        <v>990</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>907</v>
@@ -7674,7 +7678,7 @@
         <v>619</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>992</v>
+        <v>988</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>620</v>
@@ -7703,7 +7707,7 @@
         <v>717</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>718</v>
@@ -8368,7 +8372,7 @@
         <v>745</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>996</v>
+        <v>992</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>718</v>
@@ -8383,7 +8387,7 @@
         <v>1</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>1020</v>
+        <v>1016</v>
       </c>
       <c r="J28">
         <v>0</v>
@@ -8415,7 +8419,7 @@
         <v>1</v>
       </c>
       <c r="I29" t="s">
-        <v>976</v>
+        <v>1021</v>
       </c>
       <c r="J29">
         <v>0</v>
@@ -8447,7 +8451,7 @@
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>977</v>
+        <v>1022</v>
       </c>
       <c r="J30">
         <v>0</v>
@@ -8464,7 +8468,7 @@
         <v>748</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>997</v>
+        <v>993</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>718</v>
@@ -8479,7 +8483,7 @@
         <v>1</v>
       </c>
       <c r="I31" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="J31">
         <v>0</v>
@@ -8511,7 +8515,7 @@
         <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="J32">
         <v>0</v>
@@ -8543,7 +8547,7 @@
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="J33">
         <v>1</v>
@@ -8560,7 +8564,7 @@
         <v>751</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>998</v>
+        <v>994</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>718</v>
@@ -8575,7 +8579,7 @@
         <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="J34">
         <v>0</v>
@@ -8607,7 +8611,7 @@
         <v>1</v>
       </c>
       <c r="I35" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="J35">
         <v>0</v>
@@ -8624,7 +8628,7 @@
         <v>753</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>999</v>
+        <v>995</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>718</v>
@@ -8639,7 +8643,7 @@
         <v>1</v>
       </c>
       <c r="I36" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="J36">
         <v>0</v>
@@ -8671,7 +8675,7 @@
         <v>1</v>
       </c>
       <c r="I37" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="J37">
         <v>0</v>
@@ -8703,7 +8707,7 @@
         <v>1</v>
       </c>
       <c r="I38" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="J38">
         <v>0</v>
@@ -8720,7 +8724,7 @@
         <v>755</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1000</v>
+        <v>996</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>718</v>
@@ -8735,7 +8739,7 @@
         <v>1</v>
       </c>
       <c r="I39" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="J39">
         <v>0</v>
@@ -8767,7 +8771,7 @@
         <v>1</v>
       </c>
       <c r="I40" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="J40">
         <v>0</v>
@@ -8784,7 +8788,7 @@
         <v>758</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1001</v>
+        <v>997</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>718</v>
@@ -8799,7 +8803,7 @@
         <v>1</v>
       </c>
       <c r="I41" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="J41">
         <v>0</v>
@@ -8831,7 +8835,7 @@
         <v>1</v>
       </c>
       <c r="I42" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="J42">
         <v>0</v>
@@ -8864,7 +8868,7 @@
         <v>1</v>
       </c>
       <c r="I43" t="s">
-        <v>1011</v>
+        <v>1007</v>
       </c>
       <c r="J43" s="6">
         <v>0</v>
@@ -8896,7 +8900,7 @@
         <v>1</v>
       </c>
       <c r="I44" t="s">
-        <v>1012</v>
+        <v>1008</v>
       </c>
       <c r="J44">
         <v>0</v>
@@ -8929,7 +8933,7 @@
         <v>1</v>
       </c>
       <c r="I45" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="J45" s="6">
         <v>1</v>
@@ -8946,7 +8950,7 @@
         <v>760</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1002</v>
+        <v>998</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>718</v>
@@ -8961,7 +8965,7 @@
         <v>1</v>
       </c>
       <c r="I46" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="J46">
         <v>0</v>
@@ -8993,7 +8997,7 @@
         <v>1</v>
       </c>
       <c r="I47" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="J47">
         <v>0</v>
@@ -9025,7 +9029,7 @@
         <v>1</v>
       </c>
       <c r="I48" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="J48">
         <v>0</v>
@@ -9042,7 +9046,7 @@
         <v>959</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1010</v>
+        <v>1006</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>929</v>
@@ -9057,7 +9061,7 @@
         <v>1</v>
       </c>
       <c r="I49" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="J49">
         <v>1</v>
@@ -9074,7 +9078,7 @@
         <v>762</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1003</v>
+        <v>999</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>718</v>
@@ -9089,7 +9093,7 @@
         <v>1</v>
       </c>
       <c r="I50" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="J50">
         <v>0</v>
@@ -9122,13 +9126,13 @@
         <v>1</v>
       </c>
       <c r="I51" t="s">
-        <v>1015</v>
+        <v>1011</v>
       </c>
       <c r="J51" s="6">
         <v>0</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>1023</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="52" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -9155,13 +9159,13 @@
         <v>1</v>
       </c>
       <c r="I52" t="s">
-        <v>1014</v>
+        <v>1010</v>
       </c>
       <c r="J52" s="6">
         <v>1</v>
       </c>
       <c r="K52" s="4" t="s">
-        <v>1023</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
@@ -9172,7 +9176,7 @@
         <v>764</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1004</v>
+        <v>1000</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>718</v>
@@ -9187,7 +9191,7 @@
         <v>1</v>
       </c>
       <c r="I53" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="J53">
         <v>0</v>
@@ -9219,7 +9223,7 @@
         <v>1</v>
       </c>
       <c r="I54" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="J54">
         <v>0</v>
@@ -9251,7 +9255,7 @@
         <v>0</v>
       </c>
       <c r="I55" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="J55">
         <v>0</v>
@@ -9268,7 +9272,7 @@
         <v>766</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1005</v>
+        <v>1001</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>718</v>
@@ -9283,7 +9287,7 @@
         <v>1</v>
       </c>
       <c r="I56" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="J56">
         <v>0</v>
@@ -9315,7 +9319,7 @@
         <v>1</v>
       </c>
       <c r="I57" t="s">
-        <v>989</v>
+        <v>1023</v>
       </c>
       <c r="J57">
         <v>0</v>
@@ -9347,13 +9351,13 @@
         <v>1</v>
       </c>
       <c r="I58" t="s">
-        <v>1017</v>
+        <v>1013</v>
       </c>
       <c r="J58">
         <v>0</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>1016</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
@@ -9379,7 +9383,7 @@
         <v>1</v>
       </c>
       <c r="I59" t="s">
-        <v>990</v>
+        <v>1024</v>
       </c>
       <c r="J59">
         <v>1</v>
@@ -9396,7 +9400,7 @@
         <v>768</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1006</v>
+        <v>1002</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>718</v>
@@ -9411,7 +9415,7 @@
         <v>1</v>
       </c>
       <c r="I60" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="J60">
         <v>0</v>
@@ -9443,7 +9447,7 @@
         <v>1</v>
       </c>
       <c r="I61" t="s">
-        <v>1024</v>
+        <v>1020</v>
       </c>
       <c r="J61">
         <v>0</v>
@@ -9460,7 +9464,7 @@
         <v>770</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1007</v>
+        <v>1003</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>718</v>
@@ -9475,7 +9479,7 @@
         <v>1</v>
       </c>
       <c r="I62" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="J62">
         <v>0</v>
@@ -9507,7 +9511,7 @@
         <v>1</v>
       </c>
       <c r="I63" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="J63">
         <v>0</v>
@@ -9539,7 +9543,7 @@
         <v>1</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>1021</v>
+        <v>1017</v>
       </c>
       <c r="J64">
         <v>1</v>
@@ -9556,7 +9560,7 @@
         <v>772</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1008</v>
+        <v>1004</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>718</v>
@@ -9571,7 +9575,7 @@
         <v>1</v>
       </c>
       <c r="I65" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="J65">
         <v>0</v>
@@ -9603,7 +9607,7 @@
         <v>1</v>
       </c>
       <c r="I66" t="s">
-        <v>991</v>
+        <v>987</v>
       </c>
       <c r="J66">
         <v>0</v>
@@ -9620,7 +9624,7 @@
         <v>912</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>913</v>
@@ -9635,7 +9639,7 @@
         <v>1</v>
       </c>
       <c r="I67" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="J67">
         <v>0</v>

</xml_diff>

<commit_message>
update security type 算法
</commit_message>
<xml_diff>
--- a/data/basic_info.xlsx
+++ b/data/basic_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\trading_plan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4CC26A-202F-4FCE-A3FE-7119BC1AC5E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0711EBD9-34B9-4550-9828-B4E1DDB24C81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="375" yWindow="9630" windowWidth="13860" windowHeight="10065" tabRatio="733" activeTab="1" xr2:uid="{855E00D3-25C3-4BB2-A61F-0D95BB1AF006}"/>
+    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28590" tabRatio="733" activeTab="1" xr2:uid="{855E00D3-25C3-4BB2-A61F-0D95BB1AF006}"/>
   </bookViews>
   <sheets>
     <sheet name="acct_info" sheetId="1" r:id="rId1"/>
@@ -7614,10 +7614,10 @@
   <dimension ref="A1:K133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I60" sqref="I60"/>
+      <selection pane="bottomRight" activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7690,7 +7690,7 @@
         <v>622</v>
       </c>
       <c r="H2" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>890</v>
@@ -7719,7 +7719,7 @@
         <v>720</v>
       </c>
       <c r="H3" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>804</v>
@@ -7745,7 +7745,7 @@
         <v>622</v>
       </c>
       <c r="H4" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>626</v>
@@ -7771,7 +7771,7 @@
         <v>622</v>
       </c>
       <c r="H5" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>626</v>
@@ -7797,7 +7797,7 @@
         <v>720</v>
       </c>
       <c r="H6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>804</v>
@@ -7823,7 +7823,7 @@
         <v>615</v>
       </c>
       <c r="H7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>616</v>
@@ -7849,7 +7849,7 @@
         <v>720</v>
       </c>
       <c r="H8" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>804</v>
@@ -7875,7 +7875,7 @@
         <v>615</v>
       </c>
       <c r="H9" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>627</v>
@@ -7901,7 +7901,7 @@
         <v>720</v>
       </c>
       <c r="H10" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>804</v>
@@ -7927,7 +7927,7 @@
         <v>615</v>
       </c>
       <c r="H11" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>628</v>
@@ -7953,7 +7953,7 @@
         <v>615</v>
       </c>
       <c r="H12" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>629</v>
@@ -7979,7 +7979,7 @@
         <v>720</v>
       </c>
       <c r="H13" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>804</v>
@@ -8005,7 +8005,7 @@
         <v>615</v>
       </c>
       <c r="H14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>630</v>
@@ -8031,7 +8031,7 @@
         <v>720</v>
       </c>
       <c r="H15" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>804</v>
@@ -8057,7 +8057,7 @@
         <v>615</v>
       </c>
       <c r="H16" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>626</v>
@@ -8083,7 +8083,7 @@
         <v>720</v>
       </c>
       <c r="H17" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>804</v>
@@ -8109,7 +8109,7 @@
         <v>615</v>
       </c>
       <c r="H18" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>631</v>
@@ -8135,7 +8135,7 @@
         <v>720</v>
       </c>
       <c r="H19" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>804</v>
@@ -8161,7 +8161,7 @@
         <v>615</v>
       </c>
       <c r="H20" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>637</v>
@@ -8187,7 +8187,7 @@
         <v>720</v>
       </c>
       <c r="H21" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>804</v>
@@ -8213,7 +8213,7 @@
         <v>615</v>
       </c>
       <c r="H22" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>632</v>
@@ -8239,7 +8239,7 @@
         <v>720</v>
       </c>
       <c r="H23" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>804</v>
@@ -8265,7 +8265,7 @@
         <v>615</v>
       </c>
       <c r="H24" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>626</v>
@@ -8291,7 +8291,7 @@
         <v>720</v>
       </c>
       <c r="H25" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>804</v>
@@ -9665,7 +9665,7 @@
         <v>615</v>
       </c>
       <c r="H68" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I68" s="1" t="s">
         <v>626</v>
@@ -9691,7 +9691,7 @@
         <v>720</v>
       </c>
       <c r="H69" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I69" s="1" t="s">
         <v>804</v>
@@ -9717,7 +9717,7 @@
         <v>720</v>
       </c>
       <c r="H70" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I70" s="1" t="s">
         <v>804</v>
@@ -9743,7 +9743,7 @@
         <v>642</v>
       </c>
       <c r="H71" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I71" s="1" t="s">
         <v>643</v>
@@ -9769,7 +9769,7 @@
         <v>615</v>
       </c>
       <c r="H72" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I72" s="1" t="s">
         <v>626</v>
@@ -9795,7 +9795,7 @@
         <v>615</v>
       </c>
       <c r="H73" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I73" s="1" t="s">
         <v>626</v>
@@ -9821,7 +9821,7 @@
         <v>720</v>
       </c>
       <c r="H74" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I74" s="1" t="s">
         <v>804</v>
@@ -9847,7 +9847,7 @@
         <v>720</v>
       </c>
       <c r="H75" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I75" s="1" t="s">
         <v>804</v>
@@ -9873,7 +9873,7 @@
         <v>720</v>
       </c>
       <c r="H76" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I76" s="1" t="s">
         <v>804</v>
@@ -9899,7 +9899,7 @@
         <v>615</v>
       </c>
       <c r="H77" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I77" s="1" t="s">
         <v>633</v>
@@ -9925,7 +9925,7 @@
         <v>720</v>
       </c>
       <c r="H78" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I78" s="1" t="s">
         <v>804</v>
@@ -9951,7 +9951,7 @@
         <v>720</v>
       </c>
       <c r="H79" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I79" s="1" t="s">
         <v>804</v>
@@ -9977,7 +9977,7 @@
         <v>720</v>
       </c>
       <c r="H80" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I80" s="1" t="s">
         <v>804</v>
@@ -10003,7 +10003,7 @@
         <v>615</v>
       </c>
       <c r="H81" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I81" s="1" t="s">
         <v>634</v>
@@ -10029,7 +10029,7 @@
         <v>720</v>
       </c>
       <c r="H82" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I82" s="1" t="s">
         <v>804</v>
@@ -10055,7 +10055,7 @@
         <v>615</v>
       </c>
       <c r="H83" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I83" s="1" t="s">
         <v>635</v>
@@ -10081,7 +10081,7 @@
         <v>720</v>
       </c>
       <c r="H84" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I84" s="1" t="s">
         <v>804</v>
@@ -10107,7 +10107,7 @@
         <v>720</v>
       </c>
       <c r="H85" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I85" s="1" t="s">
         <v>804</v>
@@ -10133,7 +10133,7 @@
         <v>615</v>
       </c>
       <c r="H86" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I86" s="1" t="s">
         <v>626</v>
@@ -10159,7 +10159,7 @@
         <v>615</v>
       </c>
       <c r="H87" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I87" s="1" t="s">
         <v>626</v>
@@ -10185,7 +10185,7 @@
         <v>720</v>
       </c>
       <c r="H88" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I88" s="1" t="s">
         <v>804</v>
@@ -10211,7 +10211,7 @@
         <v>615</v>
       </c>
       <c r="H89" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I89" s="1" t="s">
         <v>626</v>
@@ -10237,7 +10237,7 @@
         <v>720</v>
       </c>
       <c r="H90" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I90" s="1" t="s">
         <v>804</v>
@@ -10263,7 +10263,7 @@
         <v>614</v>
       </c>
       <c r="H91" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I91" s="1" t="s">
         <v>626</v>
@@ -10289,7 +10289,7 @@
         <v>615</v>
       </c>
       <c r="H92" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I92" s="1" t="s">
         <v>626</v>
@@ -10315,7 +10315,7 @@
         <v>720</v>
       </c>
       <c r="H93" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I93" s="1" t="s">
         <v>804</v>
@@ -10341,7 +10341,7 @@
         <v>615</v>
       </c>
       <c r="H94" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I94" s="1" t="s">
         <v>626</v>
@@ -10367,7 +10367,7 @@
         <v>720</v>
       </c>
       <c r="H95" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I95" s="1" t="s">
         <v>804</v>
@@ -10393,7 +10393,7 @@
         <v>614</v>
       </c>
       <c r="H96" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I96" s="1" t="s">
         <v>626</v>
@@ -10419,7 +10419,7 @@
         <v>615</v>
       </c>
       <c r="H97" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I97" s="1" t="s">
         <v>636</v>
@@ -10428,7 +10428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>801</v>
       </c>
@@ -10445,7 +10445,7 @@
         <v>720</v>
       </c>
       <c r="H98" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I98" s="1" t="s">
         <v>804</v>
@@ -10471,7 +10471,7 @@
         <v>826</v>
       </c>
       <c r="H99" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I99" s="1" t="s">
         <v>870</v>
@@ -10497,7 +10497,7 @@
         <v>818</v>
       </c>
       <c r="H100" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I100" s="1" t="s">
         <v>871</v>
@@ -10523,7 +10523,7 @@
         <v>818</v>
       </c>
       <c r="H101" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I101" s="1" t="s">
         <v>870</v>
@@ -10549,7 +10549,7 @@
         <v>818</v>
       </c>
       <c r="H102" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I102" s="1" t="s">
         <v>870</v>
@@ -10575,7 +10575,7 @@
         <v>818</v>
       </c>
       <c r="H103" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I103" s="1" t="s">
         <v>871</v>
@@ -10601,7 +10601,7 @@
         <v>818</v>
       </c>
       <c r="H104" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I104" s="1" t="s">
         <v>870</v>
@@ -10627,7 +10627,7 @@
         <v>818</v>
       </c>
       <c r="H105" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I105" s="1" t="s">
         <v>870</v>
@@ -10653,7 +10653,7 @@
         <v>818</v>
       </c>
       <c r="H106" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I106" s="1" t="s">
         <v>871</v>
@@ -10679,7 +10679,7 @@
         <v>818</v>
       </c>
       <c r="H107" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I107" s="1" t="s">
         <v>870</v>
@@ -10705,7 +10705,7 @@
         <v>818</v>
       </c>
       <c r="H108" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I108" s="1" t="s">
         <v>872</v>
@@ -10731,7 +10731,7 @@
         <v>818</v>
       </c>
       <c r="H109" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I109" s="1" t="s">
         <v>871</v>
@@ -10757,7 +10757,7 @@
         <v>818</v>
       </c>
       <c r="H110" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I110" s="1" t="s">
         <v>871</v>
@@ -10783,7 +10783,7 @@
         <v>826</v>
       </c>
       <c r="H111" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I111" s="1" t="s">
         <v>870</v>
@@ -10809,7 +10809,7 @@
         <v>818</v>
       </c>
       <c r="H112" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I112" s="1" t="s">
         <v>874</v>
@@ -10835,7 +10835,7 @@
         <v>818</v>
       </c>
       <c r="H113" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I113" s="1" t="s">
         <v>871</v>
@@ -10861,7 +10861,7 @@
         <v>818</v>
       </c>
       <c r="H114" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I114" s="1" t="s">
         <v>875</v>
@@ -10887,7 +10887,7 @@
         <v>818</v>
       </c>
       <c r="H115" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I115" s="1" t="s">
         <v>871</v>
@@ -10913,7 +10913,7 @@
         <v>818</v>
       </c>
       <c r="H116" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I116" s="1" t="s">
         <v>870</v>
@@ -10939,7 +10939,7 @@
         <v>818</v>
       </c>
       <c r="H117" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I117" s="1" t="s">
         <v>871</v>
@@ -10965,7 +10965,7 @@
         <v>818</v>
       </c>
       <c r="H118" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I118" s="1" t="s">
         <v>870</v>
@@ -10991,7 +10991,7 @@
         <v>818</v>
       </c>
       <c r="H119" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I119" s="1" t="s">
         <v>877</v>
@@ -11017,7 +11017,7 @@
         <v>818</v>
       </c>
       <c r="H120" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I120" s="1" t="s">
         <v>871</v>
@@ -11043,7 +11043,7 @@
         <v>818</v>
       </c>
       <c r="H121" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I121" s="1" t="s">
         <v>870</v>
@@ -11069,7 +11069,7 @@
         <v>818</v>
       </c>
       <c r="H122" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I122" s="1" t="s">
         <v>871</v>
@@ -11095,7 +11095,7 @@
         <v>818</v>
       </c>
       <c r="H123" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I123" s="1" t="s">
         <v>878</v>
@@ -11121,7 +11121,7 @@
         <v>818</v>
       </c>
       <c r="H124" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I124" s="1" t="s">
         <v>879</v>
@@ -11147,7 +11147,7 @@
         <v>818</v>
       </c>
       <c r="H125" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I125" s="1" t="s">
         <v>871</v>
@@ -11173,7 +11173,7 @@
         <v>818</v>
       </c>
       <c r="H126" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I126" s="1" t="s">
         <v>871</v>
@@ -11225,7 +11225,7 @@
         <v>818</v>
       </c>
       <c r="H128" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I128" s="1" t="s">
         <v>880</v>
@@ -11251,7 +11251,7 @@
         <v>818</v>
       </c>
       <c r="H129" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I129" s="1" t="s">
         <v>881</v>
@@ -11277,7 +11277,7 @@
         <v>818</v>
       </c>
       <c r="H130" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I130" s="1" t="s">
         <v>871</v>
@@ -11303,7 +11303,7 @@
         <v>818</v>
       </c>
       <c r="H131" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I131" s="1" t="s">
         <v>871</v>
@@ -11329,7 +11329,7 @@
         <v>818</v>
       </c>
       <c r="H132" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I132" s="1" t="s">
         <v>870</v>
@@ -11355,7 +11355,7 @@
         <v>818</v>
       </c>
       <c r="H133" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I133" s="1" t="s">
         <v>870</v>

</xml_diff>